<commit_message>
got export to Excel working, working on UI
</commit_message>
<xml_diff>
--- a/main/asdf.xlsx
+++ b/main/asdf.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="100">
   <si>
     <t>Buoyancy</t>
   </si>
@@ -300,6 +300,30 @@
   </si>
   <si>
     <t>5/8" Polyester                </t>
+  </si>
+  <si>
+    <t>MillerC3                      </t>
+  </si>
+  <si>
+    <t>Drop Link                     </t>
+  </si>
+  <si>
+    <t>1" Chain                      </t>
+  </si>
+  <si>
+    <t>4 Vinies on 3/4" Polysteel    </t>
+  </si>
+  <si>
+    <t>AF36↑ w WH600+SBE37 ODO     </t>
+  </si>
+  <si>
+    <t>AF44↑ w WH150+SBE37 ODO     </t>
+  </si>
+  <si>
+    <t>SeapHox in Frame              </t>
+  </si>
+  <si>
+    <t>AR861 B2S                     </t>
   </si>
 </sst>
 </file>
@@ -617,7 +641,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G98"/>
+  <dimension ref="A1:G106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -936,11 +960,73 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7"/>
-    <row r="16" spans="1:7"/>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" t="n">
+        <v>-1.07</v>
+      </c>
+      <c r="C15" t="n">
+        <v>15</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" t="n">
+        <v>-2.007</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" t="n">
+        <v>2</v>
+      </c>
+    </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>94</v>
+      </c>
+      <c r="B17" t="n">
+        <v>-33.708</v>
+      </c>
+      <c r="C17" t="n">
+        <v>200</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -991,7 +1077,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B20" t="n">
         <v>133</v>
@@ -1014,22 +1100,22 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B21" t="n">
-        <v>161</v>
+        <v>18</v>
       </c>
       <c r="C21" t="n">
-        <v>111</v>
+        <v>60</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>75</v>
+        <v>43.2</v>
       </c>
       <c r="F21" t="n">
-        <v>0.65</v>
+        <v>1</v>
       </c>
       <c r="G21" t="n">
         <v>1</v>
@@ -1037,22 +1123,22 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B22" t="n">
-        <v>166</v>
+        <v>23</v>
       </c>
       <c r="C22" t="n">
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="D22" t="n">
         <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>75</v>
+        <v>43.2</v>
       </c>
       <c r="F22" t="n">
-        <v>0.65</v>
+        <v>1</v>
       </c>
       <c r="G22" t="n">
         <v>1</v>
@@ -1060,19 +1146,19 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B23" t="n">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C23" t="n">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="D23" t="n">
         <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>77.5</v>
+        <v>71.1</v>
       </c>
       <c r="F23" t="n">
         <v>0.65</v>
@@ -1083,19 +1169,19 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B24" t="n">
-        <v>190</v>
+        <v>161</v>
       </c>
       <c r="C24" t="n">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="F24" t="n">
         <v>0.65</v>
@@ -1106,19 +1192,19 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B25" t="n">
-        <v>300</v>
+        <v>166</v>
       </c>
       <c r="C25" t="n">
-        <v>129</v>
+        <v>87</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>92.5</v>
+        <v>75</v>
       </c>
       <c r="F25" t="n">
         <v>0.65</v>
@@ -1129,19 +1215,19 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B26" t="n">
-        <v>435</v>
+        <v>135</v>
       </c>
       <c r="C26" t="n">
-        <v>135</v>
+        <v>90</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>102.5</v>
+        <v>77.5</v>
       </c>
       <c r="F26" t="n">
         <v>0.65</v>
@@ -1152,19 +1238,19 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B27" t="n">
-        <v>20.3</v>
+        <v>190</v>
       </c>
       <c r="C27" t="n">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D27" t="n">
         <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>32.5</v>
+        <v>86</v>
       </c>
       <c r="F27" t="n">
         <v>0.65</v>
@@ -1173,58 +1259,142 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7"/>
-    <row r="29" spans="1:7"/>
-    <row r="30" spans="1:7"/>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" t="n">
+        <v>300</v>
+      </c>
+      <c r="C28" t="n">
+        <v>129</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>92.5</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="G28" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" t="n">
+        <v>435</v>
+      </c>
+      <c r="C29" t="n">
+        <v>135</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" t="n">
+        <v>102.5</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="G29" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" t="n">
+        <v>20.3</v>
+      </c>
+      <c r="C30" t="n">
+        <v>100</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" t="n">
+        <v>32.5</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="G30" t="n">
+        <v>1</v>
+      </c>
+    </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>95</v>
+      </c>
+      <c r="B31" t="n">
+        <v>83.3</v>
+      </c>
+      <c r="C31" t="n">
+        <v>150</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1</v>
+      </c>
+      <c r="E31" t="n">
+        <v>1</v>
+      </c>
+      <c r="F31" t="n">
+        <v>1</v>
+      </c>
+      <c r="G31" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>96</v>
       </c>
       <c r="B32" t="n">
-        <v>-31.037</v>
+        <v>155.5</v>
       </c>
       <c r="C32" t="n">
-        <v>175</v>
+        <v>150</v>
       </c>
       <c r="D32" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32" t="n">
-        <v>1.35</v>
+        <v>1</v>
       </c>
       <c r="G32" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>97</v>
       </c>
       <c r="B33" t="n">
-        <v>-10.52</v>
+        <v>283</v>
       </c>
       <c r="C33" t="n">
-        <v>110</v>
+        <v>213</v>
       </c>
       <c r="D33" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F33" t="n">
-        <v>1.35</v>
+        <v>1</v>
       </c>
       <c r="G33" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1298,7 +1468,7 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B37" t="n">
         <v>131.5</v>
@@ -1321,22 +1491,22 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B38" t="n">
-        <v>229.327</v>
+        <v>-31.037</v>
       </c>
       <c r="C38" t="n">
-        <v>200</v>
+        <v>175</v>
       </c>
       <c r="D38" t="n">
-        <v>91</v>
+        <v>15</v>
       </c>
       <c r="E38" t="n">
         <v>0</v>
       </c>
       <c r="F38" t="n">
-        <v>0.65</v>
+        <v>1.35</v>
       </c>
       <c r="G38" t="n">
         <v>1</v>
@@ -1344,22 +1514,22 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B39" t="n">
-        <v>116.6</v>
+        <v>-10.52</v>
       </c>
       <c r="C39" t="n">
-        <v>150</v>
+        <v>110</v>
       </c>
       <c r="D39" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>91</v>
+        <v>0</v>
       </c>
       <c r="F39" t="n">
-        <v>0.65</v>
+        <v>1.35</v>
       </c>
       <c r="G39" t="n">
         <v>1</v>
@@ -1367,22 +1537,22 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B40" t="n">
-        <v>175.5</v>
+        <v>-10.52</v>
       </c>
       <c r="C40" t="n">
-        <v>168</v>
+        <v>110</v>
       </c>
       <c r="D40" t="n">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="E40" t="n">
         <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>0.5</v>
+        <v>1.35</v>
       </c>
       <c r="G40" t="n">
         <v>1</v>
@@ -1390,22 +1560,22 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B41" t="n">
-        <v>170.5</v>
+        <v>-8.34</v>
       </c>
       <c r="C41" t="n">
-        <v>150</v>
+        <v>117</v>
       </c>
       <c r="D41" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E41" t="n">
-        <v>91</v>
+        <v>0</v>
       </c>
       <c r="F41" t="n">
-        <v>0.65</v>
+        <v>1.35</v>
       </c>
       <c r="G41" t="n">
         <v>1</v>
@@ -1413,19 +1583,19 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B42" t="n">
-        <v>170.5</v>
+        <v>131.5</v>
       </c>
       <c r="C42" t="n">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D42" t="n">
         <v>0</v>
       </c>
       <c r="E42" t="n">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="F42" t="n">
         <v>0.65</v>
@@ -1436,19 +1606,19 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B43" t="n">
-        <v>283</v>
+        <v>131.5</v>
       </c>
       <c r="C43" t="n">
-        <v>213</v>
+        <v>143</v>
       </c>
       <c r="D43" t="n">
         <v>0</v>
       </c>
       <c r="E43" t="n">
-        <v>112</v>
+        <v>83</v>
       </c>
       <c r="F43" t="n">
         <v>0.65</v>
@@ -1459,19 +1629,19 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B44" t="n">
-        <v>254</v>
+        <v>229.327</v>
       </c>
       <c r="C44" t="n">
-        <v>213.4</v>
+        <v>200</v>
       </c>
       <c r="D44" t="n">
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="E44" t="n">
-        <v>115</v>
+        <v>0</v>
       </c>
       <c r="F44" t="n">
         <v>0.65</v>
@@ -1482,19 +1652,19 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B45" t="n">
-        <v>254</v>
+        <v>116.6</v>
       </c>
       <c r="C45" t="n">
-        <v>213</v>
+        <v>150</v>
       </c>
       <c r="D45" t="n">
         <v>0</v>
       </c>
       <c r="E45" t="n">
-        <v>115</v>
+        <v>91</v>
       </c>
       <c r="F45" t="n">
         <v>0.65</v>
@@ -1505,22 +1675,22 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B46" t="n">
-        <v>-5</v>
+        <v>175.5</v>
       </c>
       <c r="C46" t="n">
-        <v>75</v>
+        <v>168</v>
       </c>
       <c r="D46" t="n">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="E46" t="n">
         <v>0</v>
       </c>
       <c r="F46" t="n">
-        <v>1.3</v>
+        <v>0.5</v>
       </c>
       <c r="G46" t="n">
         <v>1</v>
@@ -1528,22 +1698,22 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B47" t="n">
-        <v>-17.3</v>
+        <v>170.5</v>
       </c>
       <c r="C47" t="n">
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="D47" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E47" t="n">
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="F47" t="n">
-        <v>1.3</v>
+        <v>0.65</v>
       </c>
       <c r="G47" t="n">
         <v>1</v>
@@ -1551,22 +1721,22 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B48" t="n">
-        <v>-17.3</v>
+        <v>170.5</v>
       </c>
       <c r="C48" t="n">
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="D48" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E48" t="n">
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="F48" t="n">
-        <v>1.3</v>
+        <v>0.65</v>
       </c>
       <c r="G48" t="n">
         <v>1</v>
@@ -1574,22 +1744,22 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B49" t="n">
-        <v>-18.3</v>
+        <v>283</v>
       </c>
       <c r="C49" t="n">
-        <v>75</v>
+        <v>213</v>
       </c>
       <c r="D49" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E49" t="n">
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="F49" t="n">
-        <v>1.3</v>
+        <v>0.65</v>
       </c>
       <c r="G49" t="n">
         <v>1</v>
@@ -1597,19 +1767,19 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B50" t="n">
-        <v>-1.8</v>
+        <v>254</v>
       </c>
       <c r="C50" t="n">
-        <v>50</v>
+        <v>213.4</v>
       </c>
       <c r="D50" t="n">
         <v>0</v>
       </c>
       <c r="E50" t="n">
-        <v>30</v>
+        <v>115</v>
       </c>
       <c r="F50" t="n">
         <v>0.65</v>
@@ -1620,22 +1790,22 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B51" t="n">
-        <v>67.72</v>
+        <v>254</v>
       </c>
       <c r="C51" t="n">
-        <v>130</v>
+        <v>213</v>
       </c>
       <c r="D51" t="n">
         <v>0</v>
       </c>
       <c r="E51" t="n">
-        <v>0</v>
+        <v>115</v>
       </c>
       <c r="F51" t="n">
-        <v>1.3</v>
+        <v>0.65</v>
       </c>
       <c r="G51" t="n">
         <v>1</v>
@@ -1643,16 +1813,16 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B52" t="n">
-        <v>151.72</v>
+        <v>-5</v>
       </c>
       <c r="C52" t="n">
-        <v>130</v>
+        <v>75</v>
       </c>
       <c r="D52" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E52" t="n">
         <v>0</v>
@@ -1666,47 +1836,131 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B53" t="n">
-        <v>-16.28</v>
+        <v>-17.3</v>
       </c>
       <c r="C53" t="n">
-        <v>130</v>
+        <v>75</v>
       </c>
       <c r="D53" t="n">
+        <v>13</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0</v>
+      </c>
+      <c r="F53" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="G53" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" t="s">
+        <v>51</v>
+      </c>
+      <c r="B54" t="n">
+        <v>-17.3</v>
+      </c>
+      <c r="C54" t="n">
+        <v>75</v>
+      </c>
+      <c r="D54" t="n">
+        <v>13</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0</v>
+      </c>
+      <c r="F54" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="G54" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" t="s">
+        <v>52</v>
+      </c>
+      <c r="B55" t="n">
+        <v>-18.3</v>
+      </c>
+      <c r="C55" t="n">
+        <v>75</v>
+      </c>
+      <c r="D55" t="n">
+        <v>13</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0</v>
+      </c>
+      <c r="F55" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="G55" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" t="s">
+        <v>53</v>
+      </c>
+      <c r="B56" t="n">
+        <v>-1.8</v>
+      </c>
+      <c r="C56" t="n">
         <v>50</v>
       </c>
-      <c r="E53" t="n">
-        <v>0</v>
-      </c>
-      <c r="F53" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="G53" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7"/>
-    <row r="55" spans="1:7"/>
-    <row r="56" spans="1:7"/>
+      <c r="D56" t="n">
+        <v>0</v>
+      </c>
+      <c r="E56" t="n">
+        <v>30</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="G56" t="n">
+        <v>1</v>
+      </c>
+    </row>
     <row r="57" spans="1:7">
       <c r="A57" t="s">
-        <v>57</v>
+        <v>54</v>
+      </c>
+      <c r="B57" t="n">
+        <v>67.72</v>
+      </c>
+      <c r="C57" t="n">
+        <v>130</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0</v>
+      </c>
+      <c r="F57" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="G57" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B58" t="n">
-        <v>-22</v>
+        <v>151.72</v>
       </c>
       <c r="C58" t="n">
-        <v>75</v>
+        <v>130</v>
       </c>
       <c r="D58" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E58" t="n">
         <v>0</v>
@@ -1720,16 +1974,16 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B59" t="n">
-        <v>-45</v>
+        <v>-16.28</v>
       </c>
       <c r="C59" t="n">
-        <v>75</v>
+        <v>130</v>
       </c>
       <c r="D59" t="n">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="E59" t="n">
         <v>0</v>
@@ -1743,48 +1997,48 @@
     </row>
     <row r="60" spans="1:7">
       <c r="A60" t="s">
-        <v>60</v>
+        <v>98</v>
       </c>
       <c r="B60" t="n">
-        <v>-8</v>
+        <v>-11.78</v>
       </c>
       <c r="C60" t="n">
-        <v>63.3</v>
+        <v>129</v>
       </c>
       <c r="D60" t="n">
-        <v>12.6</v>
+        <v>1</v>
       </c>
       <c r="E60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F60" t="n">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="G60" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="B61" t="n">
-        <v>-16</v>
+        <v>-22</v>
       </c>
       <c r="C61" t="n">
-        <v>63.3</v>
+        <v>83</v>
       </c>
       <c r="D61" t="n">
-        <v>25.2</v>
+        <v>1</v>
       </c>
       <c r="E61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="G61" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -1812,24 +2066,46 @@
     </row>
     <row r="63" spans="1:7"/>
     <row r="64" spans="1:7"/>
-    <row r="65" spans="1:7"/>
+    <row r="65" spans="1:7">
+      <c r="A65" t="s">
+        <v>57</v>
+      </c>
+    </row>
     <row r="66" spans="1:7">
       <c r="A66" t="s">
-        <v>63</v>
+        <v>58</v>
+      </c>
+      <c r="B66" t="n">
+        <v>-22</v>
+      </c>
+      <c r="C66" t="n">
+        <v>75</v>
+      </c>
+      <c r="D66" t="n">
+        <v>13</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0</v>
+      </c>
+      <c r="F66" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="G66" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:7">
       <c r="A67" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B67" t="n">
-        <v>-11.78</v>
+        <v>-45</v>
       </c>
       <c r="C67" t="n">
-        <v>130</v>
+        <v>75</v>
       </c>
       <c r="D67" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E67" t="n">
         <v>0</v>
@@ -1843,16 +2119,16 @@
     </row>
     <row r="68" spans="1:7">
       <c r="A68" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B68" t="n">
-        <v>-34.909</v>
+        <v>-8</v>
       </c>
       <c r="C68" t="n">
-        <v>220</v>
+        <v>63.3</v>
       </c>
       <c r="D68" t="n">
-        <v>15</v>
+        <v>12.6</v>
       </c>
       <c r="E68" t="n">
         <v>0</v>
@@ -1866,16 +2142,16 @@
     </row>
     <row r="69" spans="1:7">
       <c r="A69" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B69" t="n">
-        <v>-21</v>
+        <v>-16</v>
       </c>
       <c r="C69" t="n">
-        <v>60</v>
+        <v>63.3</v>
       </c>
       <c r="D69" t="n">
-        <v>21.5</v>
+        <v>25.2</v>
       </c>
       <c r="E69" t="n">
         <v>0</v>
@@ -1889,16 +2165,16 @@
     </row>
     <row r="70" spans="1:7">
       <c r="A70" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B70" t="n">
-        <v>-30</v>
+        <v>-7.3</v>
       </c>
       <c r="C70" t="n">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="D70" t="n">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="E70" t="n">
         <v>0</v>
@@ -1981,7 +2257,7 @@
     </row>
     <row r="74" spans="1:7">
       <c r="A74" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B74" t="n">
         <v>-2.8</v>
@@ -2004,16 +2280,16 @@
     </row>
     <row r="75" spans="1:7">
       <c r="A75" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B75" t="n">
-        <v>-13.073</v>
+        <v>-11.78</v>
       </c>
       <c r="C75" t="n">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="D75" t="n">
-        <v>6.2</v>
+        <v>20</v>
       </c>
       <c r="E75" t="n">
         <v>0</v>
@@ -2025,26 +2301,110 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:7"/>
-    <row r="77" spans="1:7"/>
-    <row r="78" spans="1:7"/>
+    <row r="76" spans="1:7">
+      <c r="A76" t="s">
+        <v>65</v>
+      </c>
+      <c r="B76" t="n">
+        <v>-34.909</v>
+      </c>
+      <c r="C76" t="n">
+        <v>220</v>
+      </c>
+      <c r="D76" t="n">
+        <v>15</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0</v>
+      </c>
+      <c r="F76" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="G76" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77" t="s">
+        <v>66</v>
+      </c>
+      <c r="B77" t="n">
+        <v>-21</v>
+      </c>
+      <c r="C77" t="n">
+        <v>60</v>
+      </c>
+      <c r="D77" t="n">
+        <v>21.5</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0</v>
+      </c>
+      <c r="F77" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="G77" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" t="s">
+        <v>67</v>
+      </c>
+      <c r="B78" t="n">
+        <v>-30</v>
+      </c>
+      <c r="C78" t="n">
+        <v>55</v>
+      </c>
+      <c r="D78" t="n">
+        <v>45</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0</v>
+      </c>
+      <c r="F78" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="G78" t="n">
+        <v>1</v>
+      </c>
+    </row>
     <row r="79" spans="1:7">
       <c r="A79" t="s">
-        <v>73</v>
+        <v>68</v>
+      </c>
+      <c r="B79" t="n">
+        <v>51</v>
+      </c>
+      <c r="C79" t="n">
+        <v>60</v>
+      </c>
+      <c r="D79" t="n">
+        <v>60</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0</v>
+      </c>
+      <c r="F79" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="G79" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c r="A80" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B80" t="n">
-        <v>-0.009</v>
+        <v>0</v>
       </c>
       <c r="C80" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D80" t="n">
-        <v>0.8</v>
+        <v>2.5</v>
       </c>
       <c r="E80" t="n">
         <v>0</v>
@@ -2053,21 +2413,21 @@
         <v>1.3</v>
       </c>
       <c r="G80" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:7">
       <c r="A81" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B81" t="n">
-        <v>0.001</v>
+        <v>-12.246</v>
       </c>
       <c r="C81" t="n">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="D81" t="n">
-        <v>0.5</v>
+        <v>10</v>
       </c>
       <c r="E81" t="n">
         <v>0</v>
@@ -2076,21 +2436,21 @@
         <v>1.3</v>
       </c>
       <c r="G81" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:7">
       <c r="A82" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B82" t="n">
-        <v>-0.009</v>
+        <v>-2.8</v>
       </c>
       <c r="C82" t="n">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="D82" t="n">
-        <v>0.7</v>
+        <v>6.2</v>
       </c>
       <c r="E82" t="n">
         <v>0</v>
@@ -2099,21 +2459,21 @@
         <v>1.3</v>
       </c>
       <c r="G82" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:7">
       <c r="A83" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B83" t="n">
-        <v>-24.879</v>
+        <v>-13.073</v>
       </c>
       <c r="C83" t="n">
         <v>100</v>
       </c>
       <c r="D83" t="n">
-        <v>5</v>
+        <v>6.2</v>
       </c>
       <c r="E83" t="n">
         <v>0</v>
@@ -2196,7 +2556,7 @@
     </row>
     <row r="87" spans="1:7">
       <c r="A87" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B87" t="n">
         <v>0.032</v>
@@ -2219,16 +2579,16 @@
     </row>
     <row r="88" spans="1:7">
       <c r="A88" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B88" t="n">
-        <v>-0.039</v>
+        <v>-0.009</v>
       </c>
       <c r="C88" t="n">
         <v>100</v>
       </c>
       <c r="D88" t="n">
-        <v>2.5</v>
+        <v>0.8</v>
       </c>
       <c r="E88" t="n">
         <v>0</v>
@@ -2237,21 +2597,21 @@
         <v>1.3</v>
       </c>
       <c r="G88" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="89" spans="1:7">
       <c r="A89" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B89" t="n">
-        <v>-0.033</v>
+        <v>0.001</v>
       </c>
       <c r="C89" t="n">
         <v>100</v>
       </c>
       <c r="D89" t="n">
-        <v>2.2</v>
+        <v>0.5</v>
       </c>
       <c r="E89" t="n">
         <v>0</v>
@@ -2260,21 +2620,21 @@
         <v>1.3</v>
       </c>
       <c r="G89" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="90" spans="1:7">
       <c r="A90" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B90" t="n">
-        <v>0.037</v>
+        <v>-0.009</v>
       </c>
       <c r="C90" t="n">
         <v>100</v>
       </c>
       <c r="D90" t="n">
-        <v>2.5</v>
+        <v>0.7</v>
       </c>
       <c r="E90" t="n">
         <v>0</v>
@@ -2283,21 +2643,21 @@
         <v>1.3</v>
       </c>
       <c r="G90" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="91" spans="1:7">
       <c r="A91" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B91" t="n">
-        <v>-0.027</v>
+        <v>-24.879</v>
       </c>
       <c r="C91" t="n">
         <v>100</v>
       </c>
       <c r="D91" t="n">
-        <v>1.9</v>
+        <v>5</v>
       </c>
       <c r="E91" t="n">
         <v>0</v>
@@ -2306,21 +2666,21 @@
         <v>1.3</v>
       </c>
       <c r="G91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:7">
       <c r="A92" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B92" t="n">
-        <v>0.001</v>
+        <v>-0.345</v>
       </c>
       <c r="C92" t="n">
         <v>100</v>
       </c>
       <c r="D92" t="n">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="E92" t="n">
         <v>0</v>
@@ -2329,21 +2689,21 @@
         <v>1.3</v>
       </c>
       <c r="G92" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:7">
       <c r="A93" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B93" t="n">
-        <v>0.001</v>
+        <v>-0.261</v>
       </c>
       <c r="C93" t="n">
         <v>100</v>
       </c>
       <c r="D93" t="n">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="E93" t="n">
         <v>0</v>
@@ -2352,21 +2712,21 @@
         <v>1.3</v>
       </c>
       <c r="G93" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:7">
       <c r="A94" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B94" t="n">
-        <v>-0.008</v>
+        <v>0.002</v>
       </c>
       <c r="C94" t="n">
         <v>100</v>
       </c>
       <c r="D94" t="n">
-        <v>0.7</v>
+        <v>1.9</v>
       </c>
       <c r="E94" t="n">
         <v>0</v>
@@ -2375,21 +2735,21 @@
         <v>1.3</v>
       </c>
       <c r="G94" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="95" spans="1:7">
       <c r="A95" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B95" t="n">
-        <v>-0.012</v>
+        <v>0.032</v>
       </c>
       <c r="C95" t="n">
         <v>100</v>
       </c>
       <c r="D95" t="n">
-        <v>0.8</v>
+        <v>2.5</v>
       </c>
       <c r="E95" t="n">
         <v>0</v>
@@ -2398,21 +2758,21 @@
         <v>1.3</v>
       </c>
       <c r="G95" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="96" spans="1:7">
       <c r="A96" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B96" t="n">
-        <v>-0.016</v>
+        <v>-0.039</v>
       </c>
       <c r="C96" t="n">
         <v>100</v>
       </c>
       <c r="D96" t="n">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E96" t="n">
         <v>0</v>
@@ -2421,21 +2781,21 @@
         <v>1.3</v>
       </c>
       <c r="G96" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="97" spans="1:7">
       <c r="A97" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B97" t="n">
-        <v>-0.031</v>
+        <v>-0.033</v>
       </c>
       <c r="C97" t="n">
         <v>100</v>
       </c>
       <c r="D97" t="n">
-        <v>1.2</v>
+        <v>2.2</v>
       </c>
       <c r="E97" t="n">
         <v>0</v>
@@ -2444,30 +2804,214 @@
         <v>1.3</v>
       </c>
       <c r="G97" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="98" spans="1:7">
       <c r="A98" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B98" t="n">
-        <v>-0.046</v>
+        <v>0.037</v>
       </c>
       <c r="C98" t="n">
         <v>100</v>
       </c>
       <c r="D98" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="E98" t="n">
+        <v>0</v>
+      </c>
+      <c r="F98" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="G98" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
+      <c r="A99" t="s">
+        <v>85</v>
+      </c>
+      <c r="B99" t="n">
+        <v>-0.027</v>
+      </c>
+      <c r="C99" t="n">
+        <v>100</v>
+      </c>
+      <c r="D99" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E99" t="n">
+        <v>0</v>
+      </c>
+      <c r="F99" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="G99" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
+      <c r="A100" t="s">
+        <v>86</v>
+      </c>
+      <c r="B100" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="C100" t="n">
+        <v>100</v>
+      </c>
+      <c r="D100" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="E100" t="n">
+        <v>0</v>
+      </c>
+      <c r="F100" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="G100" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7">
+      <c r="A101" t="s">
+        <v>75</v>
+      </c>
+      <c r="B101" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="C101" t="n">
+        <v>100</v>
+      </c>
+      <c r="D101" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E101" t="n">
+        <v>0</v>
+      </c>
+      <c r="F101" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="G101" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7">
+      <c r="A102" t="s">
+        <v>88</v>
+      </c>
+      <c r="B102" t="n">
+        <v>-0.012</v>
+      </c>
+      <c r="C102" t="n">
+        <v>100</v>
+      </c>
+      <c r="D102" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="E102" t="n">
+        <v>0</v>
+      </c>
+      <c r="F102" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="G102" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7">
+      <c r="A103" t="s">
+        <v>89</v>
+      </c>
+      <c r="B103" t="n">
+        <v>-0.016</v>
+      </c>
+      <c r="C103" t="n">
+        <v>100</v>
+      </c>
+      <c r="D103" t="n">
+        <v>1</v>
+      </c>
+      <c r="E103" t="n">
+        <v>0</v>
+      </c>
+      <c r="F103" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="G103" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7">
+      <c r="A104" t="s">
+        <v>90</v>
+      </c>
+      <c r="B104" t="n">
+        <v>-0.031</v>
+      </c>
+      <c r="C104" t="n">
+        <v>100</v>
+      </c>
+      <c r="D104" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="E104" t="n">
+        <v>0</v>
+      </c>
+      <c r="F104" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="G104" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7">
+      <c r="A105" t="s">
+        <v>91</v>
+      </c>
+      <c r="B105" t="n">
+        <v>-0.046</v>
+      </c>
+      <c r="C105" t="n">
+        <v>100</v>
+      </c>
+      <c r="D105" t="n">
         <v>16</v>
       </c>
-      <c r="E98" t="n">
-        <v>0</v>
-      </c>
-      <c r="F98" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="G98" t="n">
+      <c r="E105" t="n">
+        <v>0</v>
+      </c>
+      <c r="F105" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="G105" t="n">
         <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7">
+      <c r="A106" t="s">
+        <v>87</v>
+      </c>
+      <c r="B106" t="n">
+        <v>-0.19</v>
+      </c>
+      <c r="C106" t="n">
+        <v>100</v>
+      </c>
+      <c r="D106" t="n">
+        <v>1</v>
+      </c>
+      <c r="E106" t="n">
+        <v>1</v>
+      </c>
+      <c r="F106" t="n">
+        <v>1</v>
+      </c>
+      <c r="G106" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>